<commit_message>
fixing the bedrock model
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W513032\source\repos\volume testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098A4BAA-8CB6-44C3-BF1B-DAB0196F7C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CD16F5-2813-4D4D-9A95-9F1B7FAF3A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1425" windowWidth="22455" windowHeight="14775" xr2:uid="{F0785584-2F8E-4703-86B6-C279EDBD0035}"/>
+    <workbookView xWindow="1170" yWindow="825" windowWidth="22455" windowHeight="14775" xr2:uid="{F0785584-2F8E-4703-86B6-C279EDBD0035}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Can you summarize the plot of a popular movie?</t>
   </si>
   <si>
-    <t>question_id</t>
-  </si>
-  <si>
     <t>Question</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>What are some tips for testing LLM?</t>
+  </si>
+  <si>
+    <t>question-id</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,10 +435,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -454,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -486,7 +486,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>